<commit_message>
work on db filling orm readme
</commit_message>
<xml_diff>
--- a/data/sample_data.xlsx
+++ b/data/sample_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\heroku-postgres-flow\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1CEDFB-F85A-49D2-BB63-1756D0DE3F32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56297E7-EF82-4163-9131-561A7CCF6788}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sensoren" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
   <si>
     <t>sensor</t>
   </si>
@@ -441,7 +441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -561,10 +561,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC85EDBB-375A-4D8A-806B-5F3EE5FC34DA}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,45 +597,23 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -649,7 +627,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>